<commit_message>
create a dummy test file for every c-file
</commit_message>
<xml_diff>
--- a/input/pm/requirements.xlsx
+++ b/input/pm/requirements.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21727"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{169E43D8-4A99-4D47-899D-0327994A742C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95532A30-6D1C-4469-B49E-7584B788E35D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24465" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -562,7 +562,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -581,6 +581,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -594,7 +600,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -607,6 +613,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -891,8 +900,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G168"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A140" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A168"/>
+    <sheetView tabSelected="1" topLeftCell="A79" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2034,7 +2043,7 @@
       <c r="A139">
         <v>138</v>
       </c>
-      <c r="B139" s="3" t="s">
+      <c r="B139" s="6" t="s">
         <v>124</v>
       </c>
     </row>
@@ -2114,7 +2123,7 @@
       <c r="A149">
         <v>148</v>
       </c>
-      <c r="B149" s="3" t="s">
+      <c r="B149" s="6" t="s">
         <v>150</v>
       </c>
     </row>
@@ -2122,7 +2131,7 @@
       <c r="A150">
         <v>149</v>
       </c>
-      <c r="B150" s="3" t="s">
+      <c r="B150" s="6" t="s">
         <v>151</v>
       </c>
     </row>
@@ -2130,7 +2139,7 @@
       <c r="A151">
         <v>150</v>
       </c>
-      <c r="B151" s="3" t="s">
+      <c r="B151" s="6" t="s">
         <v>152</v>
       </c>
     </row>
@@ -2138,7 +2147,7 @@
       <c r="A152">
         <v>151</v>
       </c>
-      <c r="B152" s="3" t="s">
+      <c r="B152" s="6" t="s">
         <v>153</v>
       </c>
     </row>
@@ -2146,7 +2155,7 @@
       <c r="A153">
         <v>152</v>
       </c>
-      <c r="B153" s="3" t="s">
+      <c r="B153" s="6" t="s">
         <v>154</v>
       </c>
     </row>
@@ -2154,7 +2163,7 @@
       <c r="A154">
         <v>153</v>
       </c>
-      <c r="B154" s="3" t="s">
+      <c r="B154" s="6" t="s">
         <v>155</v>
       </c>
     </row>
@@ -2162,7 +2171,7 @@
       <c r="A155">
         <v>154</v>
       </c>
-      <c r="B155" s="3" t="s">
+      <c r="B155" s="6" t="s">
         <v>156</v>
       </c>
     </row>
@@ -2170,7 +2179,7 @@
       <c r="A156">
         <v>155</v>
       </c>
-      <c r="B156" s="3" t="s">
+      <c r="B156" s="6" t="s">
         <v>157</v>
       </c>
     </row>
@@ -2178,7 +2187,7 @@
       <c r="A157">
         <v>156</v>
       </c>
-      <c r="B157" s="3" t="s">
+      <c r="B157" s="6" t="s">
         <v>158</v>
       </c>
     </row>
@@ -2186,7 +2195,7 @@
       <c r="A158">
         <v>157</v>
       </c>
-      <c r="B158" s="3" t="s">
+      <c r="B158" s="6" t="s">
         <v>159</v>
       </c>
     </row>
@@ -2194,7 +2203,7 @@
       <c r="A159">
         <v>158</v>
       </c>
-      <c r="B159" s="3" t="s">
+      <c r="B159" s="6" t="s">
         <v>160</v>
       </c>
     </row>

</xml_diff>